<commit_message>
2022 / Work in progress
</commit_message>
<xml_diff>
--- a/formats/excel/MCO/2022/Formats RSA 22.xlsx
+++ b/formats/excel/MCO/2022/Formats RSA 22.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumepressiat/Documents/Developpements/Github/formats_pmeasyr/formats/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumepressiat/Documents/Developpements/Github/formats_pmeasyr/formats/excel/MCO/2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E446F119-845B-EB43-AA4E-A4C05EE6AA40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127D0553-B75B-344D-A0BB-F6576C9FE3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="26740" windowHeight="16700" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="181">
   <si>
     <t>position</t>
   </si>
@@ -570,13 +570,19 @@
   </si>
   <si>
     <t>FILLER6</t>
+  </si>
+  <si>
+    <t>Non Programmé (NP)</t>
+  </si>
+  <si>
+    <t>ADNP75</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -593,6 +599,12 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -635,13 +647,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -956,10 +969,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F90"/>
+  <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2609,49 +2622,49 @@
       <c r="A83">
         <v>206</v>
       </c>
-      <c r="B83" s="1" t="s">
-        <v>177</v>
+      <c r="B83" s="4" t="s">
+        <v>180</v>
       </c>
       <c r="C83" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D83">
         <v>0</v>
       </c>
-      <c r="E83" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F83" s="2"/>
+      <c r="E83" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>210</v>
-      </c>
-      <c r="B84" t="s">
-        <v>133</v>
-      </c>
-      <c r="C84">
-        <v>2</v>
+        <v>207</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C84" s="1">
+        <v>3</v>
       </c>
       <c r="D84">
         <v>0</v>
       </c>
-      <c r="E84" t="s">
-        <v>7</v>
-      </c>
-      <c r="F84" t="s">
-        <v>165</v>
-      </c>
+      <c r="E84" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F84" s="2"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B85" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C85">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D85">
         <v>0</v>
@@ -2660,15 +2673,15 @@
         <v>7</v>
       </c>
       <c r="F85" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B86" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C86">
         <v>6</v>
@@ -2680,38 +2693,38 @@
         <v>7</v>
       </c>
       <c r="F86" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="B87" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C87">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D87">
         <v>0</v>
       </c>
       <c r="E87" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="F87" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B88" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C88">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -2720,34 +2733,54 @@
         <v>35</v>
       </c>
       <c r="F88" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B89" t="s">
-        <v>178</v>
+        <v>137</v>
       </c>
       <c r="C89">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D89">
         <v>0</v>
       </c>
       <c r="E89" t="s">
-        <v>7</v>
+        <v>35</v>
+      </c>
+      <c r="F89" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90">
+        <v>233</v>
+      </c>
+      <c r="B90" t="s">
+        <v>178</v>
+      </c>
+      <c r="C90">
+        <v>15</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91">
         <v>248</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B91" t="s">
         <v>138</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E91" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>